<commit_message>
Se agrega job de lectura de precios
</commit_message>
<xml_diff>
--- a/server/management/src/main/resources/LISTA PRECIOS.xlsx
+++ b/server/management/src/main/resources/LISTA PRECIOS.xlsx
@@ -19,27 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Artículo</t>
   </si>
   <si>
     <t>Precio</t>
-  </si>
-  <si>
-    <t>37.000</t>
-  </si>
-  <si>
-    <t>31.200</t>
-  </si>
-  <si>
-    <t>29.655</t>
-  </si>
-  <si>
-    <t>31.105</t>
-  </si>
-  <si>
-    <t>37.699</t>
   </si>
 </sst>
 </file>
@@ -98,16 +83,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,20 +396,20 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="4"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -436,7 +417,7 @@
       <c r="A2" s="2">
         <v>990</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="2">
         <v>41800</v>
       </c>
     </row>
@@ -444,7 +425,7 @@
       <c r="A3" s="2">
         <v>994</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>44000</v>
       </c>
     </row>
@@ -452,31 +433,31 @@
       <c r="A4" s="2">
         <v>2556</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>2</v>
+      <c r="B4" s="2">
+        <v>37000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2564</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>3</v>
+      <c r="B5" s="2">
+        <v>31200</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2565</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>3</v>
+      <c r="B6" s="2">
+        <v>333333</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4006</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="2">
         <v>31000</v>
       </c>
     </row>
@@ -484,40 +465,40 @@
       <c r="A8" s="2">
         <v>4007</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>4</v>
+      <c r="B8" s="2">
+        <v>29655</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2822</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>5</v>
+      <c r="B9" s="2">
+        <v>31105</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2824</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>5</v>
+      <c r="B10" s="2">
+        <v>31105</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>2578</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>6</v>
+      <c r="B11" s="2">
+        <v>37699</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2579</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>6</v>
+      <c r="B12" s="2">
+        <v>37699</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregar dockerfile y listas
</commit_message>
<xml_diff>
--- a/server/management/src/main/resources/LISTA PRECIOS.xlsx
+++ b/server/management/src/main/resources/LISTA PRECIOS.xlsx
@@ -393,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,6 +501,14 @@
         <v>37699</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B13" s="2">
+        <v>79000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agrega ejecucion de jobs
</commit_message>
<xml_diff>
--- a/server/management/src/main/resources/LISTA PRECIOS.xlsx
+++ b/server/management/src/main/resources/LISTA PRECIOS.xlsx
@@ -396,7 +396,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +498,7 @@
         <v>2579</v>
       </c>
       <c r="B12" s="2">
-        <v>37699</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -506,7 +506,7 @@
         <v>1024</v>
       </c>
       <c r="B13" s="2">
-        <v>79000</v>
+        <v>100000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>